<commit_message>
[New] Specify threshold for TF-IDF values
</commit_message>
<xml_diff>
--- a/output/output-edges.xlsx
+++ b/output/output-edges.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="297">
   <si>
     <t>Source</t>
   </si>
@@ -118,6 +118,18 @@
     <t>during</t>
   </si>
   <si>
+    <t>expenses</t>
+  </si>
+  <si>
+    <t>decision</t>
+  </si>
+  <si>
+    <t>expenses-&gt;decision</t>
+  </si>
+  <si>
+    <t>associated with</t>
+  </si>
+  <si>
     <t>experts</t>
   </si>
   <si>
@@ -127,6 +139,27 @@
     <t>is seen by</t>
   </si>
   <si>
+    <t>backsliding</t>
+  </si>
+  <si>
+    <t>experts-&gt;backsliding</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>backsliding-&gt;point</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>effort</t>
+  </si>
+  <si>
+    <t>part-&gt;effort</t>
+  </si>
+  <si>
     <t>technology</t>
   </si>
   <si>
@@ -325,6 +358,24 @@
     <t>may cause</t>
   </si>
   <si>
+    <t>coalition</t>
+  </si>
+  <si>
+    <t>organizations</t>
+  </si>
+  <si>
+    <t>coalition-&gt;organizations</t>
+  </si>
+  <si>
+    <t>move</t>
+  </si>
+  <si>
+    <t>step</t>
+  </si>
+  <si>
+    <t>move-&gt;step</t>
+  </si>
+  <si>
     <t>type</t>
   </si>
   <si>
@@ -358,6 +409,18 @@
     <t>can cause</t>
   </si>
   <si>
+    <t>leaders</t>
+  </si>
+  <si>
+    <t>populations</t>
+  </si>
+  <si>
+    <t>leaders-&gt;populations</t>
+  </si>
+  <si>
+    <t>assured their</t>
+  </si>
+  <si>
     <t>contrary</t>
   </si>
   <si>
@@ -388,6 +451,45 @@
     <t>stays on</t>
   </si>
   <si>
+    <t>panacea</t>
+  </si>
+  <si>
+    <t>ills</t>
+  </si>
+  <si>
+    <t>panacea-&gt;ills</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>passage</t>
+  </si>
+  <si>
+    <t>passage-&gt;law</t>
+  </si>
+  <si>
+    <t>mikosz</t>
+  </si>
+  <si>
+    <t>ifes</t>
+  </si>
+  <si>
+    <t>mikosz-&gt;ifes</t>
+  </si>
+  <si>
+    <t>works for</t>
+  </si>
+  <si>
+    <t>building</t>
+  </si>
+  <si>
+    <t>societies</t>
+  </si>
+  <si>
+    <t>building-&gt;societies</t>
+  </si>
+  <si>
     <t>turkey</t>
   </si>
   <si>
@@ -463,9 +565,6 @@
     <t>exercise-&gt;eu</t>
   </si>
   <si>
-    <t>for</t>
-  </si>
-  <si>
     <t>masses</t>
   </si>
   <si>
@@ -601,6 +700,12 @@
     <t>risks</t>
   </si>
   <si>
+    <t>expenses-&gt;risks</t>
+  </si>
+  <si>
+    <t>would be coupled with</t>
+  </si>
+  <si>
     <t>risks-&gt;benefits</t>
   </si>
   <si>
@@ -623,6 +728,15 @@
   </si>
   <si>
     <t>talking</t>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>islam</t>
+  </si>
+  <si>
+    <t>river-&gt;islam</t>
   </si>
   <si>
     <t>threat</t>
@@ -1122,7 +1236,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1317,16 +1431,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -1334,16 +1448,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1351,16 +1465,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1368,16 +1482,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1385,16 +1499,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>47</v>
       </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1402,16 +1516,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
         <v>50</v>
-      </c>
-      <c r="B17" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" t="s">
-        <v>53</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1419,16 +1533,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
-        <v>54</v>
-      </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1436,16 +1550,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1453,16 +1567,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
-        <v>61</v>
-      </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1470,16 +1584,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" t="s">
-        <v>66</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1487,16 +1601,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
         <v>67</v>
-      </c>
-      <c r="D22" t="s">
-        <v>44</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1504,16 +1618,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -1521,16 +1635,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1538,7 +1652,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>75</v>
@@ -1547,7 +1661,7 @@
         <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1555,16 +1669,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>78</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1581,7 +1695,7 @@
         <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1589,16 +1703,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1606,16 +1720,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1623,16 +1737,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>17</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D30" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1640,16 +1754,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
+        <v>90</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1657,16 +1771,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>92</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1674,16 +1788,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1694,13 +1808,13 @@
         <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D34" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1708,10 +1822,10 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>100</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
         <v>101</v>
@@ -1725,16 +1839,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" t="s">
         <v>103</v>
       </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>104</v>
-      </c>
-      <c r="D36" t="s">
-        <v>15</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1742,16 +1856,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
         <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1762,13 +1876,13 @@
         <v>5</v>
       </c>
       <c r="B38" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1776,16 +1890,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D39" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1793,16 +1907,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>17</v>
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1810,16 +1924,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1827,16 +1941,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" t="s">
         <v>5</v>
       </c>
-      <c r="B42" t="s">
-        <v>100</v>
-      </c>
       <c r="C42" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="D42" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1844,16 +1958,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1864,13 +1978,13 @@
         <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1878,16 +1992,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>5</v>
       </c>
       <c r="C45" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D45" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1895,16 +2009,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C46" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D46" t="s">
-        <v>123</v>
+        <v>11</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1912,16 +2026,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>15</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1929,16 +2043,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
         <v>129</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>130</v>
-      </c>
-      <c r="D48" t="s">
-        <v>131</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -1946,7 +2060,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
         <v>132</v>
@@ -1963,16 +2077,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="C50" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -1980,16 +2094,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D51" t="s">
-        <v>49</v>
+        <v>110</v>
       </c>
       <c r="E51">
         <v>1</v>
@@ -1997,16 +2111,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
         <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="E52">
         <v>1</v>
@@ -2014,16 +2128,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C53" t="s">
         <v>143</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>144</v>
-      </c>
-      <c r="C53" t="s">
-        <v>145</v>
-      </c>
-      <c r="D53" t="s">
-        <v>56</v>
       </c>
       <c r="E53">
         <v>1</v>
@@ -2031,16 +2145,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B54" t="s">
         <v>146</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>147</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>148</v>
-      </c>
-      <c r="D54" t="s">
-        <v>149</v>
       </c>
       <c r="E54">
         <v>1</v>
@@ -2048,13 +2162,13 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" t="s">
         <v>150</v>
-      </c>
-      <c r="B55" t="s">
-        <v>151</v>
-      </c>
-      <c r="C55" t="s">
-        <v>152</v>
       </c>
       <c r="D55" t="s">
         <v>15</v>
@@ -2065,16 +2179,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
+        <v>151</v>
+      </c>
+      <c r="B56" t="s">
+        <v>152</v>
+      </c>
+      <c r="C56" t="s">
         <v>153</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>154</v>
-      </c>
-      <c r="C56" t="s">
-        <v>155</v>
-      </c>
-      <c r="D56" t="s">
-        <v>156</v>
       </c>
       <c r="E56">
         <v>1</v>
@@ -2082,16 +2196,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" t="s">
+        <v>156</v>
+      </c>
+      <c r="C57" t="s">
         <v>157</v>
       </c>
-      <c r="B57" t="s">
-        <v>158</v>
-      </c>
-      <c r="C57" t="s">
-        <v>159</v>
-      </c>
       <c r="D57" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -2099,16 +2213,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
+        <v>158</v>
+      </c>
+      <c r="B58" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" t="s">
         <v>160</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>161</v>
-      </c>
-      <c r="C58" t="s">
-        <v>162</v>
-      </c>
-      <c r="D58" t="s">
-        <v>163</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2116,16 +2230,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
+        <v>162</v>
+      </c>
+      <c r="B59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" t="s">
         <v>164</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>165</v>
-      </c>
-      <c r="C59" t="s">
-        <v>166</v>
-      </c>
-      <c r="D59" t="s">
-        <v>167</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -2133,16 +2247,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
         <v>168</v>
-      </c>
-      <c r="B60" t="s">
-        <v>169</v>
-      </c>
-      <c r="C60" t="s">
-        <v>170</v>
-      </c>
-      <c r="D60" t="s">
-        <v>171</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -2150,16 +2264,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>19</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D61" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -2167,16 +2281,16 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>171</v>
       </c>
       <c r="C62" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D62" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -2184,16 +2298,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>173</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C63" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D63" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E63">
         <v>1</v>
@@ -2201,16 +2315,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D64" t="s">
-        <v>183</v>
+        <v>67</v>
       </c>
       <c r="E64">
         <v>1</v>
@@ -2218,16 +2332,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B65" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C65" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D65" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2235,16 +2349,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
+        <v>183</v>
+      </c>
+      <c r="B66" t="s">
+        <v>184</v>
+      </c>
+      <c r="C66" t="s">
         <v>185</v>
       </c>
-      <c r="B66" t="s">
-        <v>132</v>
-      </c>
-      <c r="C66" t="s">
-        <v>188</v>
-      </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -2252,16 +2366,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>128</v>
+        <v>186</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C67" t="s">
+        <v>188</v>
+      </c>
+      <c r="D67" t="s">
         <v>189</v>
-      </c>
-      <c r="D67" t="s">
-        <v>15</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -2278,7 +2392,7 @@
         <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>193</v>
+        <v>148</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -2286,16 +2400,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
+        <v>193</v>
+      </c>
+      <c r="B69" t="s">
         <v>194</v>
-      </c>
-      <c r="B69" t="s">
-        <v>151</v>
       </c>
       <c r="C69" t="s">
         <v>195</v>
       </c>
       <c r="D69" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
       <c r="E69">
         <v>1</v>
@@ -2303,16 +2417,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B70" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C70" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
       <c r="E70">
         <v>1</v>
@@ -2320,16 +2434,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D71" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2337,16 +2451,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B72" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="C72" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D72" t="s">
-        <v>49</v>
+        <v>207</v>
       </c>
       <c r="E72">
         <v>1</v>
@@ -2354,16 +2468,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="B73" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="C73" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D73" t="s">
-        <v>208</v>
+        <v>107</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -2371,16 +2485,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="B74" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D74" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E74">
         <v>1</v>
@@ -2388,16 +2502,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B75" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C75" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D75" t="s">
-        <v>49</v>
+        <v>216</v>
       </c>
       <c r="E75">
         <v>1</v>
@@ -2405,16 +2519,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="B76" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C76" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="D76" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="E76">
         <v>1</v>
@@ -2422,16 +2536,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="C77" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D77" t="s">
-        <v>211</v>
+        <v>148</v>
       </c>
       <c r="E77">
         <v>1</v>
@@ -2439,16 +2553,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C78" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D78" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="E78">
         <v>1</v>
@@ -2456,16 +2570,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C79" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D79" t="s">
-        <v>11</v>
+        <v>226</v>
       </c>
       <c r="E79">
         <v>1</v>
@@ -2473,16 +2587,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>224</v>
+        <v>34</v>
       </c>
       <c r="B80" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C80" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D80" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="E80">
         <v>1</v>
@@ -2490,16 +2604,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B81" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="C81" t="s">
         <v>230</v>
       </c>
       <c r="D81" t="s">
-        <v>15</v>
+        <v>107</v>
       </c>
       <c r="E81">
         <v>1</v>
@@ -2516,7 +2630,7 @@
         <v>233</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="E82">
         <v>1</v>
@@ -2533,7 +2647,7 @@
         <v>236</v>
       </c>
       <c r="D83" t="s">
-        <v>15</v>
+        <v>237</v>
       </c>
       <c r="E83">
         <v>1</v>
@@ -2541,13 +2655,13 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C84" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D84" t="s">
         <v>15</v>
@@ -2558,16 +2672,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B85" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C85" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D85" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
       <c r="E85">
         <v>1</v>
@@ -2575,16 +2689,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B86" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C86" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D86" t="s">
-        <v>131</v>
+        <v>246</v>
       </c>
       <c r="E86">
         <v>1</v>
@@ -2592,16 +2706,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>124</v>
+        <v>244</v>
       </c>
       <c r="B87" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C87" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D87" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E87">
         <v>1</v>
@@ -2609,16 +2723,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B88" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C88" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D88" t="s">
-        <v>149</v>
+        <v>60</v>
       </c>
       <c r="E88">
         <v>1</v>
@@ -2626,16 +2740,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>124</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C89" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="D89" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E89">
         <v>1</v>
@@ -2643,16 +2757,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>12</v>
+        <v>254</v>
       </c>
       <c r="B90" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="C90" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D90" t="s">
-        <v>15</v>
+        <v>249</v>
       </c>
       <c r="E90">
         <v>1</v>
@@ -2660,16 +2774,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>132</v>
+        <v>256</v>
       </c>
       <c r="B91" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C91" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D91" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E91">
         <v>1</v>
@@ -2677,18 +2791,239 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B92" t="s">
-        <v>242</v>
+        <v>260</v>
       </c>
       <c r="C92" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="D92" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>262</v>
+      </c>
+      <c r="B93" t="s">
+        <v>263</v>
+      </c>
+      <c r="C93" t="s">
+        <v>264</v>
+      </c>
+      <c r="D93" t="s">
+        <v>265</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>266</v>
+      </c>
+      <c r="B94" t="s">
+        <v>267</v>
+      </c>
+      <c r="C94" t="s">
+        <v>268</v>
+      </c>
+      <c r="D94" t="s">
         <v>15</v>
       </c>
-      <c r="E92">
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>269</v>
+      </c>
+      <c r="B95" t="s">
+        <v>270</v>
+      </c>
+      <c r="C95" t="s">
+        <v>271</v>
+      </c>
+      <c r="D95" t="s">
+        <v>15</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>272</v>
+      </c>
+      <c r="B96" t="s">
+        <v>273</v>
+      </c>
+      <c r="C96" t="s">
+        <v>274</v>
+      </c>
+      <c r="D96" t="s">
+        <v>15</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>269</v>
+      </c>
+      <c r="B97" t="s">
+        <v>275</v>
+      </c>
+      <c r="C97" t="s">
+        <v>276</v>
+      </c>
+      <c r="D97" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>277</v>
+      </c>
+      <c r="B98" t="s">
+        <v>278</v>
+      </c>
+      <c r="C98" t="s">
+        <v>279</v>
+      </c>
+      <c r="D98" t="s">
+        <v>110</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>280</v>
+      </c>
+      <c r="B99" t="s">
+        <v>281</v>
+      </c>
+      <c r="C99" t="s">
+        <v>282</v>
+      </c>
+      <c r="D99" t="s">
+        <v>165</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>158</v>
+      </c>
+      <c r="B100" t="s">
+        <v>283</v>
+      </c>
+      <c r="C100" t="s">
+        <v>284</v>
+      </c>
+      <c r="D100" t="s">
+        <v>285</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>286</v>
+      </c>
+      <c r="B101" t="s">
+        <v>287</v>
+      </c>
+      <c r="C101" t="s">
+        <v>288</v>
+      </c>
+      <c r="D101" t="s">
+        <v>148</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" t="s">
+        <v>158</v>
+      </c>
+      <c r="B102" t="s">
+        <v>289</v>
+      </c>
+      <c r="C102" t="s">
+        <v>290</v>
+      </c>
+      <c r="D102" t="s">
+        <v>291</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" t="s">
+        <v>166</v>
+      </c>
+      <c r="C103" t="s">
+        <v>292</v>
+      </c>
+      <c r="D103" t="s">
+        <v>15</v>
+      </c>
+      <c r="E103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
+      <c r="A104" t="s">
+        <v>166</v>
+      </c>
+      <c r="B104" t="s">
+        <v>293</v>
+      </c>
+      <c r="C104" t="s">
+        <v>294</v>
+      </c>
+      <c r="D104" t="s">
+        <v>110</v>
+      </c>
+      <c r="E104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" t="s">
+        <v>295</v>
+      </c>
+      <c r="B105" t="s">
+        <v>280</v>
+      </c>
+      <c r="C105" t="s">
+        <v>296</v>
+      </c>
+      <c r="D105" t="s">
+        <v>15</v>
+      </c>
+      <c r="E105">
         <v>1</v>
       </c>
     </row>

</xml_diff>